<commit_message>
[FIX] 13/10/2024: ajuste no arquivo de parâmetros para cte, para não lançar mais ISS, devido a uma mudança de campo no Oracle, decorrente de uma atualização de sistema. O campo está vindo protegido e, por conta disso, estava ocasionando em muitas falhas.
</commit_message>
<xml_diff>
--- a/Data/Parametrização RPA.xlsx
+++ b/Data/Parametrização RPA.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rpa0DHLEARQ1\Documents\UiPath\RPA_Oracle\dhl-dtentry-oracle\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rpa0DHLEARQ1\Documents\UiPath\RPA_Oracle\PROD\dhl-dtentry-oracle\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{766E4A3A-F7F4-4FBF-9005-86A193E32ED3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20610" windowHeight="6450" firstSheet="20" activeTab="23"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="19" activeTab="24" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Completa" sheetId="1" r:id="rId1"/>
@@ -788,7 +789,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -976,16 +977,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1296,7 +1297,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C139"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2840,13 +2841,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C139"/>
+  <autoFilter ref="A1:C139" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3052,7 +3053,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3375,7 +3376,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3698,7 +3699,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4122,7 +4123,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4546,7 +4547,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4795,7 +4796,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5044,7 +5045,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5291,7 +5292,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5540,7 +5541,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5703,7 +5704,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5730,11 +5731,11 @@
       <c r="C1" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -5969,7 +5970,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6132,7 +6133,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6349,7 +6350,7 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6565,7 +6566,7 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6781,11 +6782,11 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6935,7 +6936,7 @@
         <v>53</v>
       </c>
       <c r="C12" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>62</v>
@@ -7080,7 +7081,7 @@
       <c r="B22" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="C22" s="24" t="s">
+      <c r="C22" s="23" t="s">
         <v>243</v>
       </c>
     </row>
@@ -7116,11 +7117,11 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7270,7 +7271,7 @@
         <v>59</v>
       </c>
       <c r="C12" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>62</v>
@@ -7450,7 +7451,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7669,7 +7670,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7887,7 +7888,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8106,7 +8107,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8324,7 +8325,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8530,7 +8531,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8736,7 +8737,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8939,4 +8940,10 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{736915f3-2f02-4945-8997-f2963298db46}" enabled="1" method="Standard" siteId="{cd99fef8-1cd3-4a2a-9bdf-15531181d65e}" contentBits="1" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
[NEW] 31/01/2025: parametrização de mensgaens para atualizar o PPD
</commit_message>
<xml_diff>
--- a/Data/Parametrização RPA.xlsx
+++ b/Data/Parametrização RPA.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rpa0DHLEARQ1\Documents\UiPath\RPA_Oracle\PROD\dhl-dtentry-oracle\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rpa0DHLEARQ1\Documents\UiPath\RPA_Oracle\dhl-dtentry-oracle\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{766E4A3A-F7F4-4FBF-9005-86A193E32ED3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F12AD80-ADA6-4068-8F57-477FB308476F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="19" activeTab="24" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7121,7 +7121,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7271,7 +7271,7 @@
         <v>59</v>
       </c>
       <c r="C12" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>62</v>

</xml_diff>